<commit_message>
mudanca no layout e testes
</commit_message>
<xml_diff>
--- a/atividadeform/planilha_preços.xlsx
+++ b/atividadeform/planilha_preços.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -33,11 +33,21 @@
     </font>
     <font>
       <name val="Arial"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <i val="1"/>
+      <color rgb="00505050"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
       <b val="1"/>
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -47,6 +57,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="006495ED"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00dbe5f1"/>
       </patternFill>
     </fill>
     <fill>
@@ -85,11 +105,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -457,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,15 +562,254 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n"/>
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>CAIXA DE PASSAGEM DE SOBREPOR 120x120x7,5CM</t>
+        </is>
+      </c>
       <c r="B2" s="2" t="n"/>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="2" t="n"/>
-      <c r="E2" s="2" t="n"/>
-      <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="n"/>
-      <c r="H2" s="3">
-        <f> SUM(H2:H1)</f>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Furukawa</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Nucleo</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>13/05/2020</t>
+        </is>
+      </c>
+      <c r="H2" s="5">
+        <f> E2*F2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Câmera mini Bullet</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>DS-2CD2012-I</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>Hikvision</t>
+        </is>
+      </c>
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>Hikvision</t>
+        </is>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>329.9</v>
+      </c>
+      <c r="G3" s="7" t="inlineStr">
+        <is>
+          <t>07/05/2020</t>
+        </is>
+      </c>
+      <c r="H3" s="9">
+        <f> E3*F3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ELETRODUTO GALVANIZADO A FOGO DE 1"</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n"/>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Ferro Norte</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Matec</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>17/07/2020</t>
+        </is>
+      </c>
+      <c r="H4" s="5">
+        <f> E4*F4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>ELETRODUTO PVC RÍGIDO DE ½” ANTICHAMA</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="n"/>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>Ferro Norte</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>Matec</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>32</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="G5" s="7" t="inlineStr">
+        <is>
+          <t>15/05/2020</t>
+        </is>
+      </c>
+      <c r="H5" s="9">
+        <f> E5*F5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Guia de cabo</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>furukawa</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>Matec</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>18/11/1991</t>
+        </is>
+      </c>
+      <c r="H6" s="5">
+        <f> E6*F6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>Patch Cord cat 6</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>Furukawa</t>
+        </is>
+      </c>
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>Engecopi</t>
+        </is>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>45</v>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="G7" s="7" t="inlineStr">
+        <is>
+          <t>01/05/2020</t>
+        </is>
+      </c>
+      <c r="H7" s="9">
+        <f> E7*F7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Switch POE 16 Portas</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>DS-7716/7732NI-K4/16P</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>Hikvision</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>Hikvision</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>800</v>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>15/12/2019</t>
+        </is>
+      </c>
+      <c r="H8" s="5">
+        <f> E8*F8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="n"/>
+      <c r="B9" s="10" t="n"/>
+      <c r="C9" s="10" t="n"/>
+      <c r="D9" s="10" t="n"/>
+      <c r="E9" s="10" t="n"/>
+      <c r="F9" s="10" t="n"/>
+      <c r="G9" s="10" t="n"/>
+      <c r="H9" s="11">
+        <f> SUM(H2:H8)</f>
         <v/>
       </c>
     </row>

</xml_diff>